<commit_message>
add more excel files
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/template.xlsx
+++ b/src/main/webapp/book/template.xlsx
@@ -62,13 +62,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FF7FF7ED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -97,6 +97,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7FF7ED"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -371,7 +376,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>